<commit_message>
Fixed the order of samples to be the same as the genetic covariance matrix.
</commit_message>
<xml_diff>
--- a/ClimVarMod.xlsx
+++ b/ClimVarMod.xlsx
@@ -890,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9696,8 +9696,8 @@
       <c r="A120" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="A2:Y123">
-    <sortCondition ref="A2:A123"/>
+  <sortState ref="A2:Y120">
+    <sortCondition ref="A2:A120"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>